<commit_message>
Updated tool features and priority rankings
</commit_message>
<xml_diff>
--- a/tool-strategy-features.xlsx
+++ b/tool-strategy-features.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cdm\niem\planning\tool-strategy\2019-01-21-tool-strategy-F2F\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E343A412-0D2F-4BD1-A039-FB947A0AAE53}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC5B10C5-39E4-4CBD-8002-201FD60CB479}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11325" xr2:uid="{308433C3-95F1-4641-9D39-999A5EB8508A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="248">
   <si>
     <t>Scenario Planning</t>
   </si>
@@ -150,18 +150,12 @@
     <t>Check QA and conformance on individual extension components</t>
   </si>
   <si>
-    <t>Run NIEM conformance validation directly on the exchange model</t>
-  </si>
-  <si>
     <t>Run NDR conformance validation on extension schemas via a new ConTesA web service and generate conformance report</t>
   </si>
   <si>
     <t>Upload artifacts</t>
   </si>
   <si>
-    <t>Grab sample data from mapping spreadsheet</t>
-  </si>
-  <si>
     <t>Create additional exchange artifacts</t>
   </si>
   <si>
@@ -219,12 +213,6 @@
     <t>Support multiple formats</t>
   </si>
   <si>
-    <t>Download model as UML</t>
-  </si>
-  <si>
-    <t>Download model as clicky diagram</t>
-  </si>
-  <si>
     <t>Component API</t>
   </si>
   <si>
@@ -243,9 +231,6 @@
     <t>Update SSGT to use the Format translator API to return JSON schema subset</t>
   </si>
   <si>
-    <t>Alternative is to skip this if JSON NIEM subsets do not provide enough value</t>
-  </si>
-  <si>
     <t>Generate MPD catalog from form data</t>
   </si>
   <si>
@@ -399,6 +384,9 @@
     <t>07.08</t>
   </si>
   <si>
+    <t>07.09</t>
+  </si>
+  <si>
     <t>07.07, 07.08</t>
   </si>
   <si>
@@ -507,9 +495,6 @@
     <t>Offline mode</t>
   </si>
   <si>
-    <t>Resyncs when Internet connection resumes</t>
-  </si>
-  <si>
     <t>Documentation for third-party developers</t>
   </si>
   <si>
@@ -558,9 +543,6 @@
     <t>Import XML schemas into model</t>
   </si>
   <si>
-    <t>Import JSON schemas into model</t>
-  </si>
-  <si>
     <t>Export model as mapping spreadsheet</t>
   </si>
   <si>
@@ -573,24 +555,12 @@
     <t>Manual process, but could be supported in the future with IEPD registry search</t>
   </si>
   <si>
-    <t>mid-term</t>
-  </si>
-  <si>
-    <t>?</t>
-  </si>
-  <si>
-    <t>long- term</t>
-  </si>
-  <si>
     <t>08.01</t>
   </si>
   <si>
     <t>08.02</t>
   </si>
   <si>
-    <t>08.04</t>
-  </si>
-  <si>
     <t>08.05</t>
   </si>
   <si>
@@ -672,9 +642,6 @@
     <t>Import wantlist as model</t>
   </si>
   <si>
-    <t>Wantlists do not define full component information.  Will need Component API to fill in blanks.</t>
-  </si>
-  <si>
     <t>08.07</t>
   </si>
   <si>
@@ -726,13 +693,82 @@
     <t>NDR conformance validation for older NDR 2.0 schemas</t>
   </si>
   <si>
-    <t>04.09</t>
-  </si>
-  <si>
     <t>Old ConTesA (NIEM 2.0)</t>
   </si>
   <si>
     <t>ConTesA (NIEM 3.0+)</t>
+  </si>
+  <si>
+    <t>Phase 3</t>
+  </si>
+  <si>
+    <t>04.10</t>
+  </si>
+  <si>
+    <t>Google Protocol Buffers</t>
+  </si>
+  <si>
+    <t>Phase 2</t>
+  </si>
+  <si>
+    <t>Resyncs when Internet connection resumes.  Does not need to be implemented in phase 1, but architecture has to allow for it.</t>
+  </si>
+  <si>
+    <t>Backlog</t>
+  </si>
+  <si>
+    <t>Run NIEM conformance validation on full IEPDs</t>
+  </si>
+  <si>
+    <t>IEPD registry</t>
+  </si>
+  <si>
+    <t>IEPD registry; NIEM MO review</t>
+  </si>
+  <si>
+    <t>IEPD repo; IEPD registry; NIEM MO review</t>
+  </si>
+  <si>
+    <t>Publish IEPDs</t>
+  </si>
+  <si>
+    <t>user accounts; NIEM MO business process; IEPD conf. validation</t>
+  </si>
+  <si>
+    <t>Scan all uploaded artifacts for malicious code</t>
+  </si>
+  <si>
+    <t>Export model as UML</t>
+  </si>
+  <si>
+    <t>Export model as clicky diagram</t>
+  </si>
+  <si>
+    <t>NIEM UML guidance</t>
+  </si>
+  <si>
+    <t>NIEM UML support</t>
+  </si>
+  <si>
+    <t>Additional NIEM format support</t>
+  </si>
+  <si>
+    <t>Grab sample data from mapping spreadsheet.  Capability currently available in editors like Oxygen and XMLSpy.</t>
+  </si>
+  <si>
+    <t>New tool capability.  Wantlists do not define full component information.  Will need Component API to fill in blanks.</t>
+  </si>
+  <si>
+    <t>SSGT would send the wantlist to the new tool service and get back JSON schema subset.  Alternative is to skip this if JSON NIEM subsets do not provide enough value</t>
+  </si>
+  <si>
+    <t>Check the IEPD catalog for the root element, Schematron rules, etc.</t>
+  </si>
+  <si>
+    <t>YouTube video of rigged demo</t>
+  </si>
+  <si>
+    <t>08.16</t>
   </si>
 </sst>
 </file>
@@ -921,10 +957,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3F0CDA3A-4294-4B50-8B90-20AAB3B30208}" name="Table1" displayName="Table1" ref="A1:I81" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
-  <autoFilter ref="A1:I81" xr:uid="{CDFE98F9-B2C3-4389-B8FB-E281C5F42DED}"/>
-  <sortState ref="A2:I81">
-    <sortCondition ref="C1:C81"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3F0CDA3A-4294-4B50-8B90-20AAB3B30208}" name="Table1" displayName="Table1" ref="A1:I82" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="A1:I82" xr:uid="{CDFE98F9-B2C3-4389-B8FB-E281C5F42DED}"/>
+  <sortState ref="A2:I82">
+    <sortCondition ref="C1:C82"/>
   </sortState>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{E3FAD21F-2163-40D4-99C7-560287D64058}" name="Group" dataDxfId="7"/>
@@ -1238,7 +1274,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{208E5F93-6E83-486F-8FD2-8E44382902CA}">
-  <dimension ref="A1:J81"/>
+  <dimension ref="A1:J82"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
@@ -1252,7 +1288,7 @@
     <col min="1" max="1" width="25.42578125" style="2" customWidth="1"/>
     <col min="2" max="2" width="41" style="1" customWidth="1"/>
     <col min="3" max="3" width="9.42578125" style="12" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" style="6" customWidth="1"/>
     <col min="5" max="5" width="11.140625" style="11" customWidth="1"/>
     <col min="6" max="6" width="33" style="1" customWidth="1"/>
     <col min="7" max="7" width="8" style="11" customWidth="1"/>
@@ -1263,7 +1299,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>9</v>
@@ -1299,7 +1335,7 @@
         <v>16</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="E2" s="11">
         <v>0</v>
@@ -1308,7 +1344,7 @@
         <v>19</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="J2" s="2"/>
     </row>
@@ -1320,22 +1356,22 @@
         <v>10</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="E3" s="11">
         <v>1</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="G3" s="11">
         <v>4</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="J3" s="2"/>
     </row>
@@ -1347,13 +1383,13 @@
         <v>11</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="E4" s="11">
         <v>1</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="G4" s="11">
         <v>4</v>
@@ -1366,22 +1402,22 @@
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="E5" s="11">
         <v>1</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="G5" s="11">
         <v>2</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="J5" s="2"/>
     </row>
@@ -1393,10 +1429,10 @@
         <v>14</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="E6" s="11">
         <v>0</v>
@@ -1417,10 +1453,10 @@
         <v>15</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E7" s="11">
         <v>1</v>
@@ -1442,7 +1478,7 @@
         <v>12</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E8" s="11">
         <v>1</v>
@@ -1464,7 +1500,7 @@
         <v>30</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E9" s="11">
         <v>0</v>
@@ -1483,22 +1519,22 @@
         <v>31</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E10" s="11">
         <v>0.5</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="G10" s="11">
         <v>4</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="J10" s="2"/>
     </row>
@@ -1507,17 +1543,17 @@
         <v>1</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="D11" s="12"/>
       <c r="G11" s="11" t="s">
-        <v>184</v>
+        <v>224</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="J11" s="2"/>
     </row>
@@ -1526,17 +1562,22 @@
         <v>1</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>203</v>
-      </c>
-      <c r="D12" s="12"/>
+        <v>193</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>231</v>
+      </c>
       <c r="E12" s="11">
         <v>0.5</v>
       </c>
+      <c r="G12" s="11" t="s">
+        <v>224</v>
+      </c>
       <c r="H12" s="1" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="J12" s="2"/>
     </row>
@@ -1545,10 +1586,10 @@
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="11">
@@ -1565,14 +1606,17 @@
         <v>1</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="D14" s="12"/>
+      <c r="G14" s="11" t="s">
+        <v>224</v>
+      </c>
       <c r="H14" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="J14" s="2"/>
     </row>
@@ -1584,22 +1628,22 @@
         <v>23</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E15" s="11">
         <v>1</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="G15" s="11">
         <v>6</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>21</v>
@@ -1614,10 +1658,10 @@
         <v>24</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="E16" s="11">
         <v>1</v>
@@ -1641,10 +1685,10 @@
         <v>25</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E17" s="11">
         <v>1</v>
@@ -1671,10 +1715,10 @@
         <v>40</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E18" s="11">
         <v>1</v>
@@ -1696,22 +1740,22 @@
         <v>27</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E19" s="11">
         <v>1</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>183</v>
+        <v>227</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="J19" s="2"/>
     </row>
@@ -1720,17 +1764,17 @@
         <v>2</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="11">
         <v>1</v>
       </c>
-      <c r="G20" s="11">
-        <v>99</v>
+      <c r="G20" s="11" t="s">
+        <v>224</v>
       </c>
       <c r="H20" s="1"/>
       <c r="J20" s="2"/>
@@ -1740,14 +1784,17 @@
         <v>2</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D21" s="12"/>
+      <c r="G21" s="11" t="s">
+        <v>227</v>
+      </c>
       <c r="H21" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="J21" s="2"/>
     </row>
@@ -1756,14 +1803,20 @@
         <v>2</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="D22" s="12"/>
+      <c r="F22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G22" s="11">
+        <v>7</v>
+      </c>
       <c r="H22" s="1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="J22" s="2"/>
     </row>
@@ -1775,13 +1828,13 @@
         <v>34</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E23" s="11">
         <v>1</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="G23" s="11">
         <v>4</v>
@@ -1790,7 +1843,7 @@
         <v>32</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="J23" s="2"/>
     </row>
@@ -1802,24 +1855,24 @@
         <v>33</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E24" s="11">
         <v>1</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="G24" s="11">
         <v>4</v>
       </c>
       <c r="H24" s="1"/>
       <c r="I24" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>3</v>
       </c>
@@ -1827,16 +1880,16 @@
         <v>38</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="E25" s="11">
         <v>1</v>
       </c>
-      <c r="G25" s="11">
-        <v>99</v>
+      <c r="G25" s="11" t="s">
+        <v>229</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>44</v>
+        <v>242</v>
       </c>
       <c r="J25" s="2"/>
     </row>
@@ -1848,13 +1901,13 @@
         <v>37</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E26" s="11">
         <v>1</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="G26" s="11">
         <v>5</v>
@@ -1870,13 +1923,13 @@
         <v>36</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E27" s="11">
         <v>1</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="G27" s="11">
         <v>5</v>
@@ -1889,19 +1942,19 @@
         <v>3</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E28" s="11">
         <v>1</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="G28" s="11">
         <v>5</v>
@@ -1910,7 +1963,7 @@
         <v>39</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
       <c r="J28" s="2"/>
     </row>
@@ -1919,16 +1972,19 @@
         <v>3</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>41</v>
+        <v>230</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E29" s="11">
         <v>1</v>
       </c>
+      <c r="F29" s="1" t="s">
+        <v>72</v>
+      </c>
       <c r="G29" s="11">
-        <v>99</v>
+        <v>5</v>
       </c>
       <c r="H29" s="1"/>
       <c r="J29" s="2"/>
@@ -1938,22 +1994,22 @@
         <v>3</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E30" s="11">
         <v>1</v>
       </c>
-      <c r="G30" s="11" t="s">
-        <v>182</v>
+      <c r="G30" s="11">
+        <v>2</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="J30" s="2"/>
     </row>
@@ -1962,18 +2018,18 @@
         <v>3</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="D31" s="12"/>
       <c r="G31" s="11" t="s">
-        <v>184</v>
+        <v>224</v>
       </c>
       <c r="H31" s="1"/>
       <c r="I31" s="1" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="J31" s="2"/>
     </row>
@@ -1982,16 +2038,16 @@
         <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E32" s="11">
         <v>1</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="G32" s="11">
         <v>4</v>
@@ -2004,17 +2060,17 @@
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D33" s="12"/>
       <c r="E33" s="11">
         <v>1</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="G33" s="11">
         <v>4</v>
@@ -2027,10 +2083,10 @@
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E34" s="11">
         <v>0</v>
@@ -2039,7 +2095,7 @@
         <v>19</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J34" s="2"/>
     </row>
@@ -2048,19 +2104,19 @@
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E35" s="11">
         <v>1</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="G35" s="11">
         <v>4</v>
@@ -2073,25 +2129,25 @@
         <v>4</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E36" s="11">
         <v>1</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="G36" s="11">
         <v>4</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="J36" s="2"/>
     </row>
@@ -2100,25 +2156,25 @@
         <v>4</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="E37" s="11">
         <v>1</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="G37" s="11">
         <v>5</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="J37" s="2"/>
     </row>
@@ -2127,14 +2183,14 @@
         <v>4</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D38" s="12"/>
       <c r="F38" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="G38" s="11">
         <v>5</v>
@@ -2142,64 +2198,82 @@
       <c r="H38" s="1"/>
       <c r="J38" s="2"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>110</v>
+        <v>105</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>232</v>
       </c>
       <c r="E39" s="11">
         <v>1</v>
       </c>
-      <c r="G39" s="11">
-        <v>99</v>
+      <c r="F39" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="G39" s="11" t="s">
+        <v>227</v>
       </c>
       <c r="H39" s="1"/>
       <c r="J39" s="2"/>
     </row>
-    <row r="40" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>111</v>
+        <v>106</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>233</v>
       </c>
       <c r="E40" s="11">
         <v>1</v>
       </c>
-      <c r="G40" s="11">
-        <v>99</v>
+      <c r="F40" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="G40" s="11" t="s">
+        <v>227</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="J40" s="2"/>
     </row>
-    <row r="41" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>112</v>
+        <v>107</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>235</v>
       </c>
       <c r="E41" s="11">
         <v>0.5</v>
       </c>
-      <c r="G41" s="11">
-        <v>99</v>
+      <c r="F41" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="G41" s="11" t="s">
+        <v>227</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J41" s="2"/>
     </row>
@@ -2208,16 +2282,16 @@
         <v>5</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="E42" s="11">
         <v>1</v>
       </c>
-      <c r="G42" s="11">
-        <v>99</v>
+      <c r="G42" s="11" t="s">
+        <v>224</v>
       </c>
       <c r="H42" s="1"/>
       <c r="J42" s="2"/>
@@ -2227,16 +2301,16 @@
         <v>5</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="E43" s="11">
         <v>1</v>
       </c>
-      <c r="G43" s="11">
-        <v>99</v>
+      <c r="G43" s="11" t="s">
+        <v>229</v>
       </c>
       <c r="H43" s="1"/>
       <c r="J43" s="2"/>
@@ -2246,62 +2320,62 @@
         <v>5</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="E44" s="11">
         <v>1</v>
       </c>
       <c r="G44" s="11" t="s">
-        <v>184</v>
+        <v>224</v>
       </c>
       <c r="H44" s="1"/>
       <c r="J44" s="2"/>
     </row>
     <row r="45" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E45" s="11">
         <v>1</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="G45" s="11">
         <v>1</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="J45" s="2"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D46" s="12" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E46" s="11">
         <v>1</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="G46" s="11">
         <v>1</v>
@@ -2311,22 +2385,22 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="D47" s="12" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E47" s="11">
         <v>1</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="G47" s="11">
         <v>1</v>
@@ -2336,55 +2410,61 @@
     </row>
     <row r="48" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C48" s="12" t="s">
         <v>207</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="C48" s="12" t="s">
-        <v>218</v>
       </c>
       <c r="D48" s="12"/>
       <c r="F48" s="1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="G48" s="11">
         <v>1</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="J48" s="2"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="C49" s="12" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="D49" s="12"/>
+      <c r="F49" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G49" s="11">
+        <v>1</v>
+      </c>
       <c r="H49" s="1"/>
       <c r="J49" s="2"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C50" s="12" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="E50" s="11">
         <v>1</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="G50" s="11">
         <v>4</v>
@@ -2394,13 +2474,13 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C51" s="12" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="E51" s="11">
         <v>1</v>
@@ -2414,84 +2494,82 @@
       <c r="H51" s="1"/>
       <c r="J51" s="2"/>
     </row>
-    <row r="52" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C52" s="12" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D52" s="12"/>
-      <c r="G52" s="11" t="s">
-        <v>184</v>
+      <c r="F52" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G52" s="11">
+        <v>1</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>160</v>
+        <v>228</v>
       </c>
       <c r="J52" s="2"/>
     </row>
-    <row r="53" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A53" s="13" t="s">
-        <v>63</v>
+    <row r="53" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" s="9" t="s">
+        <v>197</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>174</v>
+        <v>236</v>
       </c>
       <c r="C53" s="12" t="s">
-        <v>185</v>
-      </c>
-      <c r="E53" s="11">
-        <v>1</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>171</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="D53" s="12"/>
       <c r="G53" s="11">
         <v>2</v>
       </c>
       <c r="H53" s="1"/>
       <c r="J53" s="2"/>
     </row>
-    <row r="54" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" s="13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B54" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C54" s="12" t="s">
         <v>176</v>
       </c>
-      <c r="C54" s="12" t="s">
-        <v>186</v>
-      </c>
       <c r="E54" s="11">
         <v>1</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>179</v>
+        <v>166</v>
       </c>
       <c r="G54" s="11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H54" s="1"/>
       <c r="J54" s="2"/>
     </row>
     <row r="55" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B55" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C55" s="12" t="s">
         <v>177</v>
       </c>
-      <c r="C55" s="12" t="s">
-        <v>187</v>
-      </c>
       <c r="E55" s="11">
         <v>1</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="G55" s="11">
         <v>3</v>
@@ -2501,19 +2579,19 @@
     </row>
     <row r="56" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" s="13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="C56" s="12" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="E56" s="11">
         <v>1</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="G56" s="11">
         <v>2</v>
@@ -2521,67 +2599,73 @@
       <c r="H56" s="1"/>
       <c r="J56" s="2"/>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="C57" s="12" t="s">
-        <v>190</v>
+        <v>180</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>239</v>
       </c>
       <c r="E57" s="11">
         <v>1</v>
       </c>
-      <c r="G57" s="11">
-        <v>99</v>
+      <c r="F57" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="G57" s="11" t="s">
+        <v>227</v>
       </c>
       <c r="H57" s="1"/>
       <c r="J57" s="2"/>
     </row>
-    <row r="58" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A58" s="13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="C58" s="12" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
       <c r="D58" s="12" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="E58" s="11">
         <v>0.5</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="G58" s="11" t="s">
-        <v>183</v>
+        <v>229</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>215</v>
+        <v>243</v>
       </c>
       <c r="J58" s="2"/>
     </row>
     <row r="59" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A59" s="13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C59" s="12" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="E59" s="11">
         <v>1</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="G59" s="11">
         <v>2</v>
@@ -2591,43 +2675,43 @@
     </row>
     <row r="60" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="C60" s="12" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="E60" s="11">
         <v>1</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="G60" s="11">
         <v>3</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="J60" s="2"/>
     </row>
     <row r="61" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" s="13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C61" s="12" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="E61" s="11">
         <v>1</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="G61" s="11">
         <v>2</v>
@@ -2635,155 +2719,156 @@
       <c r="H61" s="1"/>
       <c r="J61" s="2"/>
     </row>
-    <row r="62" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="C62" s="12" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="E62" s="11">
         <v>1</v>
       </c>
+      <c r="F62" s="1" t="s">
+        <v>241</v>
+      </c>
       <c r="G62" s="11" t="s">
-        <v>182</v>
+        <v>227</v>
       </c>
       <c r="H62" s="1"/>
       <c r="J62" s="2"/>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>64</v>
+        <v>237</v>
       </c>
       <c r="C63" s="12" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="E63" s="11">
         <v>1</v>
       </c>
-      <c r="G63" s="11">
-        <v>99</v>
+      <c r="F63" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="G63" s="11" t="s">
+        <v>227</v>
       </c>
       <c r="H63" s="1"/>
       <c r="J63" s="2"/>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>65</v>
+        <v>238</v>
       </c>
       <c r="C64" s="12" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="E64" s="11">
         <v>1</v>
       </c>
-      <c r="G64" s="11">
-        <v>99</v>
+      <c r="F64" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="G64" s="11" t="s">
+        <v>227</v>
       </c>
       <c r="H64" s="1"/>
       <c r="J64" s="2"/>
     </row>
-    <row r="65" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>68</v>
+        <v>226</v>
       </c>
       <c r="C65" s="12" t="s">
-        <v>197</v>
+        <v>247</v>
       </c>
       <c r="D65" s="12"/>
-      <c r="E65" s="11">
-        <v>1</v>
-      </c>
-      <c r="F65" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="G65" s="11">
+      <c r="G65" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="H65" s="1"/>
+      <c r="J65" s="2"/>
+    </row>
+    <row r="66" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A66" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C66" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="D66" s="12"/>
+      <c r="E66" s="11">
+        <v>1</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="G66" s="11">
         <v>2</v>
       </c>
-      <c r="H65" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="J65" s="2"/>
-    </row>
-    <row r="66" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A66" s="14" t="s">
-        <v>208</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C66" s="12" t="s">
+      <c r="H66" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J66" s="2"/>
+    </row>
+    <row r="67" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A67" s="14" t="s">
         <v>198</v>
       </c>
-      <c r="E66" s="11">
-        <v>1</v>
-      </c>
-      <c r="F66" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="G66" s="11">
-        <v>6</v>
-      </c>
-      <c r="H66" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="J66" s="2"/>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A67" s="14" t="s">
-        <v>208</v>
-      </c>
       <c r="B67" s="1" t="s">
-        <v>66</v>
+        <v>125</v>
       </c>
       <c r="C67" s="12" t="s">
-        <v>199</v>
-      </c>
-      <c r="D67" s="12" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="E67" s="11">
         <v>1</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="G67" s="11">
         <v>6</v>
       </c>
-      <c r="H67" s="1"/>
+      <c r="H67" s="1" t="s">
+        <v>220</v>
+      </c>
       <c r="J67" s="2"/>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="14" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C68" s="12" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="D68" s="12" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="E68" s="11">
         <v>1</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="G68" s="11">
         <v>6</v>
@@ -2791,252 +2876,320 @@
       <c r="H68" s="1"/>
       <c r="J68" s="2"/>
     </row>
-    <row r="69" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="14" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="C69" s="12" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="D69" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="E69" s="11">
+        <v>1</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="G69" s="11">
+        <v>6</v>
+      </c>
+      <c r="H69" s="1"/>
+      <c r="J69" s="2"/>
+    </row>
+    <row r="70" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A70" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C70" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="D70" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="E70" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="G70" s="11">
+        <v>6</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J70" s="2"/>
+    </row>
+    <row r="71" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A71" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C71" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="D71" s="12"/>
+      <c r="F71" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="G71" s="11">
+        <v>3</v>
+      </c>
+      <c r="H71" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A72" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C72" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="E69" s="11">
+      <c r="D72" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="E72" s="11">
         <v>0.5</v>
       </c>
-      <c r="G69" s="11">
-        <v>99</v>
-      </c>
-      <c r="H69" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="J69" s="2"/>
-    </row>
-    <row r="70" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="14" t="s">
-        <v>208</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C70" s="12" t="s">
-        <v>229</v>
-      </c>
-      <c r="D70" s="12"/>
-      <c r="H70" s="1" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A71" s="15" t="s">
-        <v>164</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="C71" s="12" t="s">
-        <v>209</v>
-      </c>
-      <c r="D71" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="E71" s="11">
-        <v>0.5</v>
-      </c>
-      <c r="F71" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="G71" s="11">
-        <v>1</v>
-      </c>
-      <c r="H71" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="J71" s="2"/>
-    </row>
-    <row r="72" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A72" s="15" t="s">
-        <v>164</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C72" s="12" t="s">
-        <v>210</v>
-      </c>
-      <c r="D72" s="12"/>
-      <c r="E72" s="11">
-        <v>1</v>
-      </c>
       <c r="F72" s="1" t="s">
-        <v>171</v>
+        <v>76</v>
       </c>
       <c r="G72" s="11">
-        <v>2</v>
-      </c>
-      <c r="H72" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="H72" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="J72" s="2"/>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A73" s="15" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C73" s="12" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="D73" s="12"/>
       <c r="E73" s="11">
         <v>1</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>77</v>
+        <v>166</v>
       </c>
       <c r="G73" s="11">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H73" s="1"/>
+      <c r="J73" s="2"/>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="15" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C74" s="12" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="D74" s="12"/>
       <c r="E74" s="11">
         <v>1</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>180</v>
+        <v>72</v>
       </c>
       <c r="G74" s="11">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H74" s="1"/>
     </row>
-    <row r="75" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="15" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="C75" s="12" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="D75" s="12"/>
       <c r="E75" s="11">
         <v>1</v>
       </c>
       <c r="F75" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="G75" s="11">
+        <v>6</v>
+      </c>
+      <c r="H75" s="1"/>
+    </row>
+    <row r="76" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A76" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C76" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="D76" s="12"/>
+      <c r="E76" s="11">
+        <v>1</v>
+      </c>
+      <c r="F76" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G75" s="11">
+      <c r="G76" s="11">
         <v>8</v>
       </c>
-      <c r="H75" s="1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A76" s="15" t="s">
-        <v>164</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C76" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="D76" s="12"/>
-      <c r="H76" s="1"/>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A77" s="16" t="s">
-        <v>219</v>
+      <c r="H76" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A77" s="15" t="s">
+        <v>159</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C77" s="12" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="D77" s="12"/>
-      <c r="H77" s="1"/>
+      <c r="F77" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G77" s="11">
+        <v>5</v>
+      </c>
+      <c r="H77" s="1" t="s">
+        <v>245</v>
+      </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="16" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="C78" s="12" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="D78" s="12"/>
+      <c r="F78" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G78" s="11">
+        <v>1</v>
+      </c>
       <c r="H78" s="1"/>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="16" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="C79" s="12" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="D79" s="12"/>
+      <c r="F79" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G79" s="11">
+        <v>1</v>
+      </c>
       <c r="H79" s="1"/>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="16" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="C80" s="12" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="D80" s="12"/>
-      <c r="H80" s="1"/>
-    </row>
-    <row r="81" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A81" s="17" t="s">
-        <v>225</v>
+      <c r="F80" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G80" s="11">
+        <v>1</v>
+      </c>
+      <c r="H80" s="1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81" s="16" t="s">
+        <v>208</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>71</v>
+        <v>164</v>
       </c>
       <c r="C81" s="12" t="s">
-        <v>228</v>
-      </c>
-      <c r="D81" s="12" t="s">
-        <v>197</v>
-      </c>
-      <c r="E81" s="11">
+        <v>213</v>
+      </c>
+      <c r="D81" s="12"/>
+      <c r="F81" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G81" s="11">
+        <v>1</v>
+      </c>
+      <c r="H81" s="1"/>
+    </row>
+    <row r="82" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A82" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C82" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="D82" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="E82" s="11">
         <v>0.5</v>
       </c>
-      <c r="F81" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G81" s="11" t="s">
-        <v>183</v>
-      </c>
-      <c r="H81" s="1" t="s">
-        <v>72</v>
+      <c r="F82" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G82" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="H82" s="1" t="s">
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -3049,7 +3202,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E70 E73 E75 E81">
+  <conditionalFormatting sqref="E71 E74 E76 E82">
     <cfRule type="iconSet" priority="2">
       <iconSet iconSet="3Symbols" showValue="0">
         <cfvo type="percent" val="0"/>
@@ -3058,7 +3211,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E3 E5:E69 E71:E72">
+  <conditionalFormatting sqref="E72:E73 E2:E3 E5:E70">
     <cfRule type="iconSet" priority="8">
       <iconSet iconSet="3Symbols" showValue="0">
         <cfvo type="percent" val="0"/>

</xml_diff>